<commit_message>
procedimentos definidos em 23/10
</commit_message>
<xml_diff>
--- a/analise_da_evasao_estudantil/Docs Complementares/agenda_projeto.xlsx
+++ b/analise_da_evasao_estudantil/Docs Complementares/agenda_projeto.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alinefonseca/Dropbox/ENAp/Bootcamp 2023/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alinefonseca/Dropbox/Mac/Documents/GitHub/projetos-do-bootcamp-analise-de-dados-enap-2023/analise_da_evasao_estudantil/Docs Complementares/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6E3A658-8B05-4E46-BD26-50D6215B47FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36A79518-AEF2-CD44-BC68-AED82583BA62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="800" yWindow="2500" windowWidth="27840" windowHeight="16340" xr2:uid="{BF2B75C1-CFA4-0047-9E48-C6FDD79EC673}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{BF2B75C1-CFA4-0047-9E48-C6FDD79EC673}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Atividades</t>
   </si>
@@ -68,6 +68,27 @@
   </si>
   <si>
     <t>Demo Day</t>
+  </si>
+  <si>
+    <t>Comparativo 2008-2012 X 2013-2023 (marco Lei das Cotas)</t>
+  </si>
+  <si>
+    <t>Inicialmente PISM e SISU (vestibular para o período de 2008-2012)</t>
+  </si>
+  <si>
+    <t>Tirar os "cursos" ABI</t>
+  </si>
+  <si>
+    <t>Evasão por tipo de ingresso</t>
+  </si>
+  <si>
+    <t>Evasão por cota</t>
+  </si>
+  <si>
+    <t>Evasão por sexo</t>
+  </si>
+  <si>
+    <t>Evasão por curso</t>
   </si>
 </sst>
 </file>
@@ -420,24 +441,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2C8EB75-88AD-3C4B-A1F4-02B8C3F46BBC}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.5" customWidth="1"/>
     <col min="2" max="2" width="53.83203125" customWidth="1"/>
+    <col min="3" max="3" width="41.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>45218</v>
       </c>
@@ -445,7 +467,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>45219</v>
       </c>
@@ -453,31 +475,40 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>45222</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>45223</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>45224</v>
       </c>
       <c r="B6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>45225</v>
       </c>
@@ -485,36 +516,48 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>45226</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>45229</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>45230</v>
       </c>
       <c r="B10" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>45231</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>